<commit_message>
Added filter per company and excel generation
</commit_message>
<xml_diff>
--- a/DatabaseToExcel.xlsx
+++ b/DatabaseToExcel.xlsx
@@ -4,14 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="First" sheetId="1" r:id="rId1"/>
+    <sheet name="Acosta, Butler and Perez" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="New" sheetId="4" r:id="rId4"/>
-    <sheet name="Evaluation Warning" sheetId="5" r:id="rId5"/>
+    <sheet name="Evaluation Warning" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr fullCalcOnLoad="1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -36,22 +35,70 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Nihar</t>
-  </si>
-  <si>
-    <t>2023PCP5317</t>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>Specialization</t>
+  </si>
+  <si>
+    <t>10th Marks</t>
+  </si>
+  <si>
+    <t>12th Marks</t>
+  </si>
+  <si>
+    <t>CGPA</t>
+  </si>
+  <si>
+    <t>Backlogs</t>
+  </si>
+  <si>
+    <t>Red Flags</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Inna</t>
+  </si>
+  <si>
+    <t>2023PCP5321</t>
   </si>
   <si>
     <t>8050106439</t>
   </si>
   <si>
-    <t>niharkajla28@gmail.com</t>
-  </si>
-  <si>
-    <t>Ellen Degenerous</t>
-  </si>
-  <si>
-    <t>2023PCP5318</t>
+    <t>niharkajla123@gmail.com</t>
+  </si>
+  <si>
+    <t>2024-01-16</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>PG</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>SC</t>
   </si>
   <si>
     <t>Suhana Sharma</t>
@@ -63,25 +110,13 @@
     <t>niharamazon5005@gmail.com</t>
   </si>
   <si>
-    <t>Sagar Shah</t>
-  </si>
-  <si>
-    <t>2023PCP5319</t>
-  </si>
-  <si>
-    <t>niharkajla123@gmail.com</t>
-  </si>
-  <si>
-    <t>Samay Raina</t>
-  </si>
-  <si>
-    <t>2023PCP5320</t>
-  </si>
-  <si>
-    <t>Inna</t>
-  </si>
-  <si>
-    <t>2023PCP5321</t>
+    <t>2024-03-07</t>
+  </si>
+  <si>
+    <t>CSE</t>
+  </si>
+  <si>
+    <t>General</t>
   </si>
   <si>
     <t>Spire.XLS for Python</t>
@@ -587,19 +622,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultColWidthPt="48.75" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="15.8515625" widthPt="83.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.57421875" widthPt="76.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" widthPt="69" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" widthPt="82.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.28125" widthPt="138" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.57421875" widthPt="66" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.00390625" widthPt="42" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" widthPt="48" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28125" widthPt="75" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.8515625" widthPt="57" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.57421875" widthPt="34.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.421875" widthPt="49.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.28125" widthPt="54" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.421875" widthPt="49.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12.75">
+    <row r="1" spans="1:14" ht="12.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -612,89 +656,123 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="12.75">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="12.75">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="12.75">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="12.75">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="12.75">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="12.75">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="12.75">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="12.75">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -734,20 +812,6 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultColWidthPt="48.75" defaultRowHeight="12.75"/>
-  <sheetData/>
-  <printOptions/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
@@ -756,42 +820,42 @@
   <sheetData>
     <row r="1" ht="12.75">
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" ht="12.75">
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" ht="12.75">
       <c r="B4" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" ht="12.75">
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" ht="12.75">
       <c r="B7" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" ht="12.75">
       <c r="B8" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" ht="12.75">
       <c r="B10" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" ht="12.75">
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Starting work of student offers by admin page
</commit_message>
<xml_diff>
--- a/DatabaseToExcel.xlsx
+++ b/DatabaseToExcel.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Acosta, Butler and Perez" sheetId="1" r:id="rId1"/>
+    <sheet name="Alexander, Bradley and Gonzales" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Evaluation Warning" sheetId="4" r:id="rId4"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -65,58 +65,127 @@
     <t>Category</t>
   </si>
   <si>
-    <t>Inna</t>
-  </si>
-  <si>
-    <t>2023PCP5321</t>
+    <t>Nihar</t>
+  </si>
+  <si>
+    <t>2023PCP5317</t>
   </si>
   <si>
     <t>8050106439</t>
   </si>
   <si>
+    <t>niharkajla28@gmail.com</t>
+  </si>
+  <si>
+    <t>1995-10-28</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>PG</t>
+  </si>
+  <si>
+    <t>CSE</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>8.167</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Samay Raina</t>
+  </si>
+  <si>
+    <t>2023PCP5320</t>
+  </si>
+  <si>
+    <t>2023-12-07</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Suhana Sharma</t>
+  </si>
+  <si>
+    <t>2023PCP5305</t>
+  </si>
+  <si>
+    <t>niharamazon5005@gmail.com</t>
+  </si>
+  <si>
+    <t>2024-03-07</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Sagar Shah</t>
+  </si>
+  <si>
+    <t>2023PCP5319</t>
+  </si>
+  <si>
     <t>niharkajla123@gmail.com</t>
   </si>
   <si>
-    <t>2024-01-16</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>PG</t>
-  </si>
-  <si>
-    <t>CE</t>
-  </si>
-  <si>
-    <t>90</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>SC</t>
-  </si>
-  <si>
-    <t>Suhana Sharma</t>
-  </si>
-  <si>
-    <t>2023PCP5305</t>
-  </si>
-  <si>
-    <t>niharamazon5005@gmail.com</t>
-  </si>
-  <si>
-    <t>2024-03-07</t>
-  </si>
-  <si>
-    <t>CSE</t>
-  </si>
-  <si>
-    <t>General</t>
+    <t>2024-02-01</t>
+  </si>
+  <si>
+    <t>VLSI</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>8.75</t>
+  </si>
+  <si>
+    <t>OBC</t>
+  </si>
+  <si>
+    <t>Ellen Degenerous</t>
+  </si>
+  <si>
+    <t>2023PCP5318</t>
+  </si>
+  <si>
+    <t>2024-03-05</t>
+  </si>
+  <si>
+    <t>CSIS</t>
+  </si>
+  <si>
+    <t>70</t>
   </si>
   <si>
     <t>Spire.XLS for Python</t>
@@ -622,13 +691,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultColWidthPt="48.75" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.57421875" widthPt="76.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.8515625" widthPt="83.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" widthPt="69" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" widthPt="82.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.28125" widthPt="138" bestFit="1" customWidth="1"/>
@@ -716,36 +785,36 @@
         <v>22</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="N2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="12.75">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
@@ -754,25 +823,157 @@
         <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="K3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="12.75">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="12.75">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" t="s">
         <v>23</v>
       </c>
-      <c r="L3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" t="s">
-        <v>31</v>
+      <c r="K5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="12.75">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -820,42 +1021,42 @@
   <sheetData>
     <row r="1" ht="12.75">
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" ht="12.75">
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" ht="12.75">
       <c r="B4" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" ht="12.75">
       <c r="B5" s="3" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" ht="12.75">
       <c r="B7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" ht="12.75">
       <c r="B8" s="3" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" ht="12.75">
       <c r="B10" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" ht="12.75">
       <c r="B11" s="3" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added offer page code for admin
</commit_message>
<xml_diff>
--- a/DatabaseToExcel.xlsx
+++ b/DatabaseToExcel.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Alexander, Bradley and Gonzales" sheetId="1" r:id="rId1"/>
+    <sheet name="Acosta, Butler and Perez" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Evaluation Warning" sheetId="4" r:id="rId4"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -65,15 +65,66 @@
     <t>Category</t>
   </si>
   <si>
+    <t>Inna</t>
+  </si>
+  <si>
+    <t>2023PCP5321</t>
+  </si>
+  <si>
+    <t>8050106439</t>
+  </si>
+  <si>
+    <t>niharkajla123@gmail.com</t>
+  </si>
+  <si>
+    <t>2024-01-16</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>PG</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>Suhana Sharma</t>
+  </si>
+  <si>
+    <t>2023PCP5305</t>
+  </si>
+  <si>
+    <t>niharamazon5005@gmail.com</t>
+  </si>
+  <si>
+    <t>2024-03-07</t>
+  </si>
+  <si>
+    <t>CSE</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
     <t>Nihar</t>
   </si>
   <si>
     <t>2023PCP5317</t>
   </si>
   <si>
-    <t>8050106439</t>
-  </si>
-  <si>
     <t>niharkajla28@gmail.com</t>
   </si>
   <si>
@@ -83,12 +134,6 @@
     <t>Male</t>
   </si>
   <si>
-    <t>PG</t>
-  </si>
-  <si>
-    <t>CSE</t>
-  </si>
-  <si>
     <t>88</t>
   </si>
   <si>
@@ -101,52 +146,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>General</t>
-  </si>
-  <si>
-    <t>Samay Raina</t>
-  </si>
-  <si>
-    <t>2023PCP5320</t>
-  </si>
-  <si>
-    <t>2023-12-07</t>
-  </si>
-  <si>
-    <t>PS</t>
-  </si>
-  <si>
-    <t>90</t>
-  </si>
-  <si>
-    <t>95</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>Suhana Sharma</t>
-  </si>
-  <si>
-    <t>2023PCP5305</t>
-  </si>
-  <si>
-    <t>niharamazon5005@gmail.com</t>
-  </si>
-  <si>
-    <t>2024-03-07</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>9</t>
+    <t>2</t>
   </si>
   <si>
     <t>Sagar Shah</t>
@@ -155,9 +155,6 @@
     <t>2023PCP5319</t>
   </si>
   <si>
-    <t>niharkajla123@gmail.com</t>
-  </si>
-  <si>
     <t>2024-02-01</t>
   </si>
   <si>
@@ -171,21 +168,6 @@
   </si>
   <si>
     <t>OBC</t>
-  </si>
-  <si>
-    <t>Ellen Degenerous</t>
-  </si>
-  <si>
-    <t>2023PCP5318</t>
-  </si>
-  <si>
-    <t>2024-03-05</t>
-  </si>
-  <si>
-    <t>CSIS</t>
-  </si>
-  <si>
-    <t>70</t>
   </si>
   <si>
     <t>Spire.XLS for Python</t>
@@ -691,13 +673,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultColWidthPt="48.75" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="15.8515625" widthPt="83.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.57421875" widthPt="76.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" widthPt="69" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" widthPt="82.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.28125" widthPt="138" bestFit="1" customWidth="1"/>
@@ -785,36 +767,36 @@
         <v>22</v>
       </c>
       <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>24</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" t="s">
         <v>25</v>
-      </c>
-      <c r="M2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="12.75">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
@@ -823,69 +805,69 @@
         <v>20</v>
       </c>
       <c r="H3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" t="s">
         <v>31</v>
-      </c>
-      <c r="I3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="12.75">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
         <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="J4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="K4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" t="s">
         <v>41</v>
       </c>
-      <c r="L4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4" t="s">
-        <v>35</v>
-      </c>
       <c r="N4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="12.75">
@@ -899,81 +881,37 @@
         <v>16</v>
       </c>
       <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
         <v>44</v>
       </c>
-      <c r="E5" t="s">
-        <v>45</v>
-      </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
         <v>20</v>
       </c>
       <c r="H5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" t="s">
         <v>46</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" t="s">
         <v>47</v>
       </c>
-      <c r="J5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" t="s">
         <v>48</v>
-      </c>
-      <c r="L5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="12.75">
-      <c r="A6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" t="s">
-        <v>54</v>
-      </c>
-      <c r="J6" t="s">
-        <v>54</v>
-      </c>
-      <c r="K6" t="s">
-        <v>41</v>
-      </c>
-      <c r="L6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N6" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1021,42 +959,42 @@
   <sheetData>
     <row r="1" ht="12.75">
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" ht="12.75">
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" ht="12.75">
       <c r="B4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" ht="12.75">
       <c r="B5" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" ht="12.75">
       <c r="B7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" ht="12.75">
       <c r="B8" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" ht="12.75">
       <c r="B10" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" ht="12.75">
       <c r="B11" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Shown to sir for final assesment:
</commit_message>
<xml_diff>
--- a/DatabaseToExcel.xlsx
+++ b/DatabaseToExcel.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Acosta, Butler and Perez" sheetId="1" r:id="rId1"/>
+    <sheet name="Student Data" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Evaluation Warning" sheetId="4" r:id="rId4"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="68">
   <si>
     <t>Name</t>
   </si>
@@ -101,6 +101,60 @@
     <t>SC</t>
   </si>
   <si>
+    <t>Samay Raina</t>
+  </si>
+  <si>
+    <t>2023PCP5320</t>
+  </si>
+  <si>
+    <t>niharkajla28@gmail.com</t>
+  </si>
+  <si>
+    <t>2023-12-07</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Sagar Shah</t>
+  </si>
+  <si>
+    <t>2023PCP5319</t>
+  </si>
+  <si>
+    <t>2024-02-01</t>
+  </si>
+  <si>
+    <t>VLSI</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>8.75</t>
+  </si>
+  <si>
+    <t>OBC</t>
+  </si>
+  <si>
     <t>Suhana Sharma</t>
   </si>
   <si>
@@ -116,7 +170,37 @@
     <t>CSE</t>
   </si>
   <si>
-    <t>General</t>
+    <t>Ellen Degenerous</t>
+  </si>
+  <si>
+    <t>2023PCP5318</t>
+  </si>
+  <si>
+    <t>2024-03-05</t>
+  </si>
+  <si>
+    <t>CSIS</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>Nihar</t>
+  </si>
+  <si>
+    <t>2023PCP5317</t>
+  </si>
+  <si>
+    <t>1995-10-28</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>8.167</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
   <si>
     <t>Spire.XLS for Python</t>
@@ -622,13 +706,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultColWidthPt="48.75" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.57421875" widthPt="76.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.8515625" widthPt="83.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" widthPt="69" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" widthPt="82.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.28125" widthPt="138" bestFit="1" customWidth="1"/>
@@ -748,31 +832,207 @@
         <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
         <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I3" t="s">
         <v>22</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="K3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="L3" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="M3" t="s">
         <v>24</v>
       </c>
       <c r="N3" t="s">
-        <v>31</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="12.75">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="12.75">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="12.75">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="12.75">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" t="s">
+        <v>58</v>
+      </c>
+      <c r="L7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" t="s">
+        <v>59</v>
+      </c>
+      <c r="N7" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -820,42 +1080,42 @@
   <sheetData>
     <row r="1" ht="12.75">
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" ht="12.75">
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" ht="12.75">
       <c r="B4" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" ht="12.75">
       <c r="B5" s="3" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" ht="12.75">
       <c r="B7" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" ht="12.75">
       <c r="B8" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" ht="12.75">
       <c r="B10" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" ht="12.75">
       <c r="B11" s="3" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>